<commit_message>
fix bug in matrix size of willem2012 matrices
</commit_message>
<xml_diff>
--- a/data/raw/interaction_matrices/willem_2012/0_20_60/home.xlsx
+++ b/data/raw/interaction_matrices/willem_2012/0_20_60/home.xlsx
@@ -62,12 +62,11 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -83,6 +82,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,12 +132,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -153,72 +162,69 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="1" sqref="A1:D4 E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>1.00044265381733</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>1.82008177258967</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>0.0288331884650301</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.66181670270159</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>1.37148831760854</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>0.119265632685674</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>0.0254294783790366</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>0.289276580019193</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>0.752974810592319</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -236,72 +242,69 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="1" sqref="A1:D4 B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0.848828746713403</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>1.58907366450667</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>0.0243535056938586</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.577817716122383</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>1.02825818304706</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>0.0825614401140962</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>0.0214786147306194</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>0.200251241701868</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>0.48972547559494</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -319,72 +322,69 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0.011073974850819</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>0.0277085981538674</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.01007537866861</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>0.0239721200696406</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>0.00596676664768604</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="0" t="n">
+      <c r="B4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>0.0144722818363293</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>0.0402290516526274</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -402,72 +402,69 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="A1:D4 C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0.0279402096503541</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>0.067149270014713</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>0.00198836473688171</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.0244167647515775</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>0.0686996342929133</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>0.0192372558216704</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>0.00175364157687579</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>0.0466596071955905</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>0.100702795900497</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -485,72 +482,69 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topLeft" activeCell="D29" activeCellId="1" sqref="A1:D4 D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0.901651143698376</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>1.59077653332968</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>0.0172869081668737</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.578436911944543</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>1.11711744231973</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>0.0755468660989592</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>0.015246217323591</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>0.183237522529823</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>0.492278442827877</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -568,72 +562,69 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0.733611551945138</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>1.20393424394299</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>0.00837268739192384</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.437773622919257</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>0.734766182139099</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>0.0535469388618529</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>0.00738430552921986</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>0.129877107056291</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>0.433576597511855</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>